<commit_message>
Swap slope & intercept labels
</commit_message>
<xml_diff>
--- a/2025_12-18_Linearization.xlsx
+++ b/2025_12-18_Linearization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DavidFulford\Dropbox\SPEE\REP-11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6603A0-0A66-4E45-8829-177E819CC46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301E1849-A0BB-4BCC-A42D-972ABD618D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5AC488F8-9BC3-4790-B2DB-80233DD882CC}"/>
   </bookViews>
@@ -5354,9 +5354,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AK64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6071,7 +6069,7 @@
       <c r="A11" s="44"/>
       <c r="B11" s="27"/>
       <c r="C11" s="30" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11" s="52">
         <f>_qi^-_b</f>
@@ -6149,7 +6147,7 @@
       <c r="A12" s="44"/>
       <c r="B12" s="27"/>
       <c r="C12" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="52">
         <f>_Dnom*_b*D11</f>
@@ -6375,7 +6373,7 @@
       <c r="A15" s="44"/>
       <c r="B15" s="27"/>
       <c r="C15" s="30" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D15" s="51">
         <f>IF(_b=1,
@@ -6456,7 +6454,7 @@
       <c r="A16" s="44"/>
       <c r="B16" s="27"/>
       <c r="C16" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="51">
         <f>IF(_b=1,

</xml_diff>